<commit_message>
add column C and add separate rows per value in column B
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sxxx_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sxxx_vorlage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\sbider\data\export\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws_intern\planpro\repos\set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1EFE09-F387-46D8-ACCB-D0F57995F65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E9CD98-EFDE-4181-8ECC-8B101C39FFFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="50820" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sskz" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>A</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Referenziert von Objekt</t>
+  </si>
+  <si>
+    <t>Ausgabe in Plan</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -133,6 +139,19 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -140,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -167,6 +186,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -478,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AO52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScale="280" zoomScaleNormal="100" zoomScalePageLayoutView="280" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -508,7 +530,9 @@
       <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -554,6 +578,9 @@
       <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -562,12 +589,14 @@
     <row r="3" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="2:41" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7"/>
       <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B5" s="4"/>
@@ -832,9 +861,10 @@
       <c r="G52" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.19685039370078741" bottom="0.59055118110236227" header="0" footer="0"/>
@@ -843,6 +873,77 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Nicht begonnen</_Status>
+    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1034,78 +1135,48 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Version xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields">Nicht begonnen</_Status>
-    <_Revision xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <_DCDateCreated xmlns="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1177B4BE-B106-4A5F-9B8B-849CAD24B948}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947F1741-2986-4B63-8B5C-D0468C671233}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD45C59E-C13E-4B92-9551-AE1790848EFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1122,45 +1193,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947F1741-2986-4B63-8B5C-D0468C671233}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1177B4BE-B106-4A5F-9B8B-849CAD24B948}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>